<commit_message>
bug in turn functions of USLocalizer
</commit_message>
<xml_diff>
--- a/Lab4_new/tests/tests_USLocalization.xlsx
+++ b/Lab4_new/tests/tests_USLocalization.xlsx
@@ -193,10 +193,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -503,8 +503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,11 +552,11 @@
       <c r="L1" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
@@ -1878,7 +1878,7 @@
       <c r="F31">
         <v>146.03</v>
       </c>
-      <c r="G31" s="4">
+      <c r="G31" s="3">
         <f t="shared" si="0"/>
         <v>8.0699999999999932</v>
       </c>
@@ -1926,18 +1926,18 @@
       <c r="F32">
         <v>60.84</v>
       </c>
-      <c r="G32" s="4">
+      <c r="G32" s="3">
         <f t="shared" ref="G32:G51" si="4">225-(E32+F32)/2</f>
         <v>92.980000000000018</v>
       </c>
-      <c r="H32" s="4">
+      <c r="H32" s="3">
         <f t="shared" ref="H32:H51" si="5">45-(E32+F32)/2</f>
         <v>-87.019999999999982</v>
       </c>
-      <c r="I32" s="4">
+      <c r="I32" s="3">
         <v>89</v>
       </c>
-      <c r="J32" s="4">
+      <c r="J32" s="3">
         <v>180</v>
       </c>
       <c r="K32">
@@ -1962,11 +1962,11 @@
       <c r="D33">
         <v>-5</v>
       </c>
-      <c r="G33" s="4">
+      <c r="G33" s="3">
         <f t="shared" si="4"/>
         <v>225</v>
       </c>
-      <c r="H33" s="4">
+      <c r="H33" s="3">
         <f t="shared" si="5"/>
         <v>45</v>
       </c>
@@ -1975,11 +1975,11 @@
       <c r="A34">
         <v>17</v>
       </c>
-      <c r="G34" s="4">
+      <c r="G34" s="3">
         <f t="shared" si="4"/>
         <v>225</v>
       </c>
-      <c r="H34" s="4">
+      <c r="H34" s="3">
         <f t="shared" si="5"/>
         <v>45</v>
       </c>
@@ -1988,171 +1988,171 @@
       <c r="A35">
         <v>18</v>
       </c>
-      <c r="G35" s="4">
+      <c r="G35" s="3">
         <f t="shared" si="4"/>
         <v>225</v>
       </c>
-      <c r="H35" s="4">
+      <c r="H35" s="3">
         <f t="shared" si="5"/>
         <v>45</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G36" s="4">
+      <c r="G36" s="3">
         <f t="shared" si="4"/>
         <v>225</v>
       </c>
-      <c r="H36" s="4">
+      <c r="H36" s="3">
         <f t="shared" si="5"/>
         <v>45</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G37" s="4">
+      <c r="G37" s="3">
         <f t="shared" si="4"/>
         <v>225</v>
       </c>
-      <c r="H37" s="4">
+      <c r="H37" s="3">
         <f t="shared" si="5"/>
         <v>45</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G38" s="4">
+      <c r="G38" s="3">
         <f t="shared" si="4"/>
         <v>225</v>
       </c>
-      <c r="H38" s="4">
+      <c r="H38" s="3">
         <f t="shared" si="5"/>
         <v>45</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G39" s="4">
+      <c r="G39" s="3">
         <f t="shared" si="4"/>
         <v>225</v>
       </c>
-      <c r="H39" s="4">
+      <c r="H39" s="3">
         <f t="shared" si="5"/>
         <v>45</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G40" s="4">
+      <c r="G40" s="3">
         <f t="shared" si="4"/>
         <v>225</v>
       </c>
-      <c r="H40" s="4">
+      <c r="H40" s="3">
         <f t="shared" si="5"/>
         <v>45</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G41" s="4">
+      <c r="G41" s="3">
         <f t="shared" si="4"/>
         <v>225</v>
       </c>
-      <c r="H41" s="4">
+      <c r="H41" s="3">
         <f t="shared" si="5"/>
         <v>45</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G42" s="4">
+      <c r="G42" s="3">
         <f t="shared" si="4"/>
         <v>225</v>
       </c>
-      <c r="H42" s="4">
+      <c r="H42" s="3">
         <f t="shared" si="5"/>
         <v>45</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G43" s="4">
+      <c r="G43" s="3">
         <f t="shared" si="4"/>
         <v>225</v>
       </c>
-      <c r="H43" s="4">
+      <c r="H43" s="3">
         <f t="shared" si="5"/>
         <v>45</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G44" s="4">
+      <c r="G44" s="3">
         <f t="shared" si="4"/>
         <v>225</v>
       </c>
-      <c r="H44" s="4">
+      <c r="H44" s="3">
         <f t="shared" si="5"/>
         <v>45</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G45" s="4">
+      <c r="G45" s="3">
         <f t="shared" si="4"/>
         <v>225</v>
       </c>
-      <c r="H45" s="4">
+      <c r="H45" s="3">
         <f t="shared" si="5"/>
         <v>45</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G46" s="4">
+      <c r="G46" s="3">
         <f t="shared" si="4"/>
         <v>225</v>
       </c>
-      <c r="H46" s="4">
+      <c r="H46" s="3">
         <f t="shared" si="5"/>
         <v>45</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G47" s="4">
+      <c r="G47" s="3">
         <f t="shared" si="4"/>
         <v>225</v>
       </c>
-      <c r="H47" s="4">
+      <c r="H47" s="3">
         <f t="shared" si="5"/>
         <v>45</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G48" s="4">
+      <c r="G48" s="3">
         <f t="shared" si="4"/>
         <v>225</v>
       </c>
-      <c r="H48" s="4">
+      <c r="H48" s="3">
         <f t="shared" si="5"/>
         <v>45</v>
       </c>
     </row>
     <row r="49" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G49" s="4">
+      <c r="G49" s="3">
         <f t="shared" si="4"/>
         <v>225</v>
       </c>
-      <c r="H49" s="4">
+      <c r="H49" s="3">
         <f t="shared" si="5"/>
         <v>45</v>
       </c>
     </row>
     <row r="50" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G50" s="4">
+      <c r="G50" s="3">
         <f t="shared" si="4"/>
         <v>225</v>
       </c>
-      <c r="H50" s="4">
+      <c r="H50" s="3">
         <f t="shared" si="5"/>
         <v>45</v>
       </c>
     </row>
     <row r="51" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G51" s="4">
+      <c r="G51" s="3">
         <f t="shared" si="4"/>
         <v>225</v>
       </c>
-      <c r="H51" s="4">
+      <c r="H51" s="3">
         <f t="shared" si="5"/>
         <v>45</v>
       </c>

</xml_diff>